<commit_message>
Update modification to integrate canada questions
</commit_message>
<xml_diff>
--- a/canada-2017.xlsx
+++ b/canada-2017.xlsx
@@ -103,13 +103,13 @@
     <t xml:space="preserve">What percentage of your time is spent on research?</t>
   </si>
   <si>
-    <t xml:space="preserve">In an average month, how much time do you spend on what you consider to be research</t>
+    <t xml:space="preserve">In an average month, how much time do you spend on research</t>
   </si>
   <si>
     <t xml:space="preserve">time3_can</t>
   </si>
   <si>
-    <t xml:space="preserve">In an average month, how much time do you spend on research</t>
+    <t xml:space="preserve">In an average month, how much time do you spend on management</t>
   </si>
   <si>
     <t xml:space="preserve">time5_can</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">time4_can</t>
   </si>
   <si>
-    <t xml:space="preserve">In an average month, how much time do you spend on other</t>
+    <t xml:space="preserve">In an average month, how much time do you spend on other activities</t>
   </si>
   <si>
     <t xml:space="preserve">What percentage of the time you spend writing software is spent on new development/enhancement?</t>
@@ -667,7 +667,7 @@
   <dimension ref="1:56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>